<commit_message>
Backup QR Scanner data - 2025-11-18T08:35:35.915Z - Cache Bust: 1763454935915
</commit_message>
<xml_diff>
--- a/log_history/Y3_B2526_Pathology_Lab_Museum_scanner1761124432990_d98a641fbd845c0a4e67d5c3df19f56b894b356cbcff263721bcbe66e39d8538.xlsx
+++ b/log_history/Y3_B2526_Pathology_Lab_Museum_scanner1761124432990_d98a641fbd845c0a4e67d5c3df19f56b894b356cbcff263721bcbe66e39d8538.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Scanner" sheetId="1" r:id="rId1"/>
+    <sheet name="Pathology_Lab_Museum" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F127"/>
+  <dimension ref="A1:F129"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2942,9 +2942,49 @@
         <v>mona.I.hussein@med.asu.edu.eg</v>
       </c>
     </row>
+    <row r="128">
+      <c r="A128" t="str">
+        <v>244030</v>
+      </c>
+      <c r="B128" t="str">
+        <v>Pathology Lab/Museum</v>
+      </c>
+      <c r="C128" t="str">
+        <v>18/11/2025</v>
+      </c>
+      <c r="D128" t="str">
+        <v>09:38:57</v>
+      </c>
+      <c r="E128" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F128" t="str">
+        <v>mona.I.hussein@med.asu.edu.eg</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="str">
+        <v>244047</v>
+      </c>
+      <c r="B129" t="str">
+        <v>Pathology Lab/Museum</v>
+      </c>
+      <c r="C129" t="str">
+        <v>18/11/2025</v>
+      </c>
+      <c r="D129" t="str">
+        <v>09:39:03</v>
+      </c>
+      <c r="E129" t="str">
+        <v>Scan</v>
+      </c>
+      <c r="F129" t="str">
+        <v>mona.I.hussein@med.asu.edu.eg</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F127"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F129"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>